<commit_message>
Pruebas de Sistema Actualizado
Se agregaron nuevas pruebas de sistema
</commit_message>
<xml_diff>
--- a/QA.xlsx
+++ b/QA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerardo Villalobos\Desktop\Aseguramiento de Software\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E20AE677-051E-4CE1-8E71-378E6090C303}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28BB5A60-984B-4CE0-8ECD-7B1AA4114C79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="110">
   <si>
     <t>Pruebas del sistema</t>
   </si>
@@ -90,21 +90,6 @@
     <t>Crear post</t>
   </si>
   <si>
-    <t>Titulo, descripción e imagen</t>
-  </si>
-  <si>
-    <t>Sin titulo, descripción e imagen</t>
-  </si>
-  <si>
-    <t>Titulo, sin descripción e imagen</t>
-  </si>
-  <si>
-    <t>Titulo, descripción e sin imagen</t>
-  </si>
-  <si>
-    <t>Titulo, descripción e imagen sin valores</t>
-  </si>
-  <si>
     <t>No aplica</t>
   </si>
   <si>
@@ -114,19 +99,262 @@
     <t>Post realizado con éxito</t>
   </si>
   <si>
-    <t>Solo titulo</t>
-  </si>
-  <si>
-    <t>Solo descripción</t>
-  </si>
-  <si>
-    <t>Solo imagen</t>
-  </si>
-  <si>
     <t>Error</t>
   </si>
   <si>
-    <t xml:space="preserve">Error </t>
+    <t>Crear cuenta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todos los espacios vacios </t>
+  </si>
+  <si>
+    <t>Mensaje de Error</t>
+  </si>
+  <si>
+    <t>Rellenar los espacios correctamente</t>
+  </si>
+  <si>
+    <t>Registro de cuenta rechazado</t>
+  </si>
+  <si>
+    <t>Creación de cuenta</t>
+  </si>
+  <si>
+    <t>Usuario repetido</t>
+  </si>
+  <si>
+    <t>Usuario ya existe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solo nombre </t>
+  </si>
+  <si>
+    <t>Solo apellido</t>
+  </si>
+  <si>
+    <t>Solo fecha de nacimiento</t>
+  </si>
+  <si>
+    <t>Solo usuario</t>
+  </si>
+  <si>
+    <t>Solo contraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solo confirmación de contraseña </t>
+  </si>
+  <si>
+    <t>Solo nombre y apellido</t>
+  </si>
+  <si>
+    <t>Solo nombre y fecha de nacimiento</t>
+  </si>
+  <si>
+    <t>Solo nombre y usuario</t>
+  </si>
+  <si>
+    <t>Solo nombre y contraseña</t>
+  </si>
+  <si>
+    <t>Solo nombre y confirmación de contraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Solo apellido y fecha de nacimiento</t>
+  </si>
+  <si>
+    <t>Solo apellido y usuario</t>
+  </si>
+  <si>
+    <t>Solo apellido y contraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solo apellido y confirmación de contraseña </t>
+  </si>
+  <si>
+    <t>Solo fecha de nacimiento y usuario</t>
+  </si>
+  <si>
+    <t>Solo fecha de nacimiento y contraseña</t>
+  </si>
+  <si>
+    <t>Solo fecha de nacimiento y confirmación de contraseña</t>
+  </si>
+  <si>
+    <t>Solo usuario y contraseña</t>
+  </si>
+  <si>
+    <t>Solo usuario y confirmación de contraseña</t>
+  </si>
+  <si>
+    <t>Solo contraseña y confirmación de contraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todo llenado correctamente pero contraseña y confirmación diferente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha con formato invalido </t>
+  </si>
+  <si>
+    <t>Contraseñas no son iguales</t>
+  </si>
+  <si>
+    <t>Titulo, descripción e imagen (pública)</t>
+  </si>
+  <si>
+    <t>Sin titulo, descripción e imagen (pública)</t>
+  </si>
+  <si>
+    <t>Titulo, sin descripción e imagen (pública)</t>
+  </si>
+  <si>
+    <t>Titulo, descripción y sin imagen (pública)</t>
+  </si>
+  <si>
+    <t>Solo titulo (pública)</t>
+  </si>
+  <si>
+    <t>Solo descripción (pública)</t>
+  </si>
+  <si>
+    <t>Solo imagen (pública)</t>
+  </si>
+  <si>
+    <t>Titulo, descripción e imagen (privada)</t>
+  </si>
+  <si>
+    <t>Sin titulo, descripción e imagen (privada)</t>
+  </si>
+  <si>
+    <t>Titulo, sin descripción e imagen (privada)</t>
+  </si>
+  <si>
+    <t>Titulo, descripción y sin imagen (privada)</t>
+  </si>
+  <si>
+    <t>Solo titulo (privada)</t>
+  </si>
+  <si>
+    <t>Solo descripción (privada)</t>
+  </si>
+  <si>
+    <t>Solo imagen (privada)</t>
+  </si>
+  <si>
+    <t>Agregar amigo</t>
+  </si>
+  <si>
+    <t>Agregar amigo nuevo</t>
+  </si>
+  <si>
+    <t>Agregar amigo existente</t>
+  </si>
+  <si>
+    <t>Nos agrega amigo existente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nos agrega amigo nuevo </t>
+  </si>
+  <si>
+    <t>Cerrar sesión</t>
+  </si>
+  <si>
+    <t>Cerrar sesión sin hacer post</t>
+  </si>
+  <si>
+    <t>Cerrar sesión haciendo post</t>
+  </si>
+  <si>
+    <t>El usuario esté logueado</t>
+  </si>
+  <si>
+    <t>Cierra sesión</t>
+  </si>
+  <si>
+    <t>Cierra sesión y se guarda el post</t>
+  </si>
+  <si>
+    <t>Cierra sesión con éxito</t>
+  </si>
+  <si>
+    <t>Likes</t>
+  </si>
+  <si>
+    <t>Dar clic al icono de like</t>
+  </si>
+  <si>
+    <t>Dar clic al icono de dislike</t>
+  </si>
+  <si>
+    <t>Dar like a publicación pública</t>
+  </si>
+  <si>
+    <t>Dar like a publicación privada</t>
+  </si>
+  <si>
+    <t>Quitar like a publicación pública</t>
+  </si>
+  <si>
+    <t>Quitar like a publicación privada</t>
+  </si>
+  <si>
+    <t>Guardar likes de publicación pública</t>
+  </si>
+  <si>
+    <t>Guardar likes de publicación privada</t>
+  </si>
+  <si>
+    <t>Guardar dislikes de publicación pública</t>
+  </si>
+  <si>
+    <t>Guardar dislikes de publicación privada</t>
+  </si>
+  <si>
+    <t>Ser amigo</t>
+  </si>
+  <si>
+    <t>Visualizar publicación pública</t>
+  </si>
+  <si>
+    <t>Visualizar publicación privada</t>
+  </si>
+  <si>
+    <t>Guardar like a la publicación</t>
+  </si>
+  <si>
+    <t>Like guardado con éxito</t>
+  </si>
+  <si>
+    <t>Quitar like a la publicación</t>
+  </si>
+  <si>
+    <t>Like quitado con éxito</t>
+  </si>
+  <si>
+    <t>Guardar likes de la publicación</t>
+  </si>
+  <si>
+    <t>Likes guardados con éxito</t>
+  </si>
+  <si>
+    <t>Guardar dislikes de la publicación</t>
+  </si>
+  <si>
+    <t>Dislikes guardados con éxito</t>
+  </si>
+  <si>
+    <t>Publicación existente</t>
+  </si>
+  <si>
+    <t>Publicación existente y amistad</t>
+  </si>
+  <si>
+    <t>Visualizar la publicación</t>
+  </si>
+  <si>
+    <t>Publicación visualizada con éxito</t>
   </si>
 </sst>
 </file>
@@ -458,19 +686,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H15"/>
+  <dimension ref="B2:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E15"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -562,69 +790,44 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -632,13 +835,16 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" t="s">
-        <v>33</v>
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -646,13 +852,16 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -660,13 +869,16 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -674,16 +886,721 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
         <v>31</v>
       </c>
-      <c r="E15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="D31" t="s">
         <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" t="s">
+        <v>29</v>
+      </c>
+      <c r="H36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" t="s">
+        <v>29</v>
+      </c>
+      <c r="H37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" t="s">
+        <v>29</v>
+      </c>
+      <c r="G53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>72</v>
+      </c>
+      <c r="C56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" t="s">
+        <v>85</v>
+      </c>
+      <c r="F61" t="s">
+        <v>98</v>
+      </c>
+      <c r="G61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" t="s">
+        <v>88</v>
+      </c>
+      <c r="D62" t="s">
+        <v>85</v>
+      </c>
+      <c r="E62" t="s">
+        <v>95</v>
+      </c>
+      <c r="F62" t="s">
+        <v>98</v>
+      </c>
+      <c r="G62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" t="s">
+        <v>89</v>
+      </c>
+      <c r="D63" t="s">
+        <v>86</v>
+      </c>
+      <c r="F63" t="s">
+        <v>100</v>
+      </c>
+      <c r="G63" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64" t="s">
+        <v>86</v>
+      </c>
+      <c r="F64" t="s">
+        <v>100</v>
+      </c>
+      <c r="G64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65" t="s">
+        <v>91</v>
+      </c>
+      <c r="F65" t="s">
+        <v>102</v>
+      </c>
+      <c r="G65" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66" t="s">
+        <v>92</v>
+      </c>
+      <c r="F66" t="s">
+        <v>102</v>
+      </c>
+      <c r="G66" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>84</v>
+      </c>
+      <c r="C67" t="s">
+        <v>93</v>
+      </c>
+      <c r="F67" t="s">
+        <v>104</v>
+      </c>
+      <c r="G67" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>84</v>
+      </c>
+      <c r="C68" t="s">
+        <v>94</v>
+      </c>
+      <c r="F68" t="s">
+        <v>104</v>
+      </c>
+      <c r="G68" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>96</v>
+      </c>
+      <c r="E70" t="s">
+        <v>106</v>
+      </c>
+      <c r="F70" t="s">
+        <v>108</v>
+      </c>
+      <c r="G70" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>97</v>
+      </c>
+      <c r="E71" t="s">
+        <v>107</v>
+      </c>
+      <c r="F71" t="s">
+        <v>108</v>
+      </c>
+      <c r="G71" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>